<commit_message>
Support date item for save.
</commit_message>
<xml_diff>
--- a/samples/testdata/save.xlsx
+++ b/samples/testdata/save.xlsx
@@ -26,13 +26,18 @@
     <t>あいう</t>
   </si>
   <si>
-    <t>Sat Oct 13 2012 12:40:06 GMT+0900 (JST)</t>
+    <t>2012-10-15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="GENERAL" numFmtId="165"/>
+    <numFmt formatCode="YYYY/MM/DD" numFmtId="166"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>

</xml_diff>